<commit_message>
ALICE calculations are done and so is the variance minimization for the 50MeV stack
</commit_message>
<xml_diff>
--- a/A0_unc_persent.xlsx
+++ b/A0_unc_persent.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{8E561148-20FF-1445-8691-D79058C33EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12B8E85C-E1B4-1840-A60B-4254BBB4C3A2}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{8E561148-20FF-1445-8691-D79058C33EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A2A6B98-0110-A34D-8B29-CE3A6D82DA72}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{F987D640-AF71-2948-8B84-AD1C60931213}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="20320" windowHeight="14920" xr2:uid="{F987D640-AF71-2948-8B84-AD1C60931213}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">Product </t>
-  </si>
-  <si>
-    <t>96Nb</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Zr01</t>
   </si>
@@ -75,6 +69,99 @@
   </si>
   <si>
     <t>This file contains relative uncertanties for all the products seen in different foils</t>
+  </si>
+  <si>
+    <t>87NB</t>
+  </si>
+  <si>
+    <t>89NB</t>
+  </si>
+  <si>
+    <t>90NB</t>
+  </si>
+  <si>
+    <t>95NB</t>
+  </si>
+  <si>
+    <t>95NBm</t>
+  </si>
+  <si>
+    <t>96NB</t>
+  </si>
+  <si>
+    <t>85Y</t>
+  </si>
+  <si>
+    <t>86Y</t>
+  </si>
+  <si>
+    <t>86Ym</t>
+  </si>
+  <si>
+    <t>87Y</t>
+  </si>
+  <si>
+    <t>87Ym</t>
+  </si>
+  <si>
+    <t>88Y</t>
+  </si>
+  <si>
+    <t>89Ym</t>
+  </si>
+  <si>
+    <t>90Ym</t>
+  </si>
+  <si>
+    <t>92Y</t>
+  </si>
+  <si>
+    <t>91Y</t>
+  </si>
+  <si>
+    <t>89ZR</t>
+  </si>
+  <si>
+    <t>88ZR</t>
+  </si>
+  <si>
+    <t>95ZR</t>
+  </si>
+  <si>
+    <t>Ni01</t>
+  </si>
+  <si>
+    <t>Ni02</t>
+  </si>
+  <si>
+    <t>Ni03</t>
+  </si>
+  <si>
+    <t>Ni04</t>
+  </si>
+  <si>
+    <t>Ni05</t>
+  </si>
+  <si>
+    <t>52MN</t>
+  </si>
+  <si>
+    <t>54MN</t>
+  </si>
+  <si>
+    <t>55CO</t>
+  </si>
+  <si>
+    <t>56CO</t>
+  </si>
+  <si>
+    <t>57CO</t>
+  </si>
+  <si>
+    <t>58CO</t>
+  </si>
+  <si>
+    <t>60CO</t>
   </si>
 </sst>
 </file>
@@ -142,6 +229,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -441,74 +532,495 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C214A759-CA15-BB43-B154-32249697E9E6}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <f>7403.30342215441/376019.094733061*100</f>
+        <v>1.9688636895980178</v>
+      </c>
+      <c r="C6">
+        <f>18765.4699830039/566363.868799972*100</f>
+        <v>3.313323998362522</v>
+      </c>
+      <c r="D6">
+        <f>10823.6115950715/261004.638627906*100</f>
+        <v>4.1469039216969161</v>
+      </c>
+      <c r="E6">
+        <f>42.9103375595412/456.016559801807*100</f>
+        <v>9.4098200245602488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
         <f xml:space="preserve"> 91.9875605863194/2697.41549709611*100</f>
         <v>3.4102110218224881</v>
       </c>
-      <c r="C4">
+      <c r="C9">
         <f xml:space="preserve"> 182.973236703185/6172.65955620562*100</f>
         <v>2.9642528481784605</v>
       </c>
-      <c r="D4">
+      <c r="D9">
         <f xml:space="preserve"> 448.032136409645/19932.065856578*100</f>
         <v>2.2477957861140871</v>
       </c>
-      <c r="E4">
+      <c r="E9">
         <f>91.3007759181304/5027.55983919886*100</f>
         <v>1.8160057530549285</v>
       </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="1"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="1"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="1"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="1"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="1"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="1"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
calibration for all distances are fixed. I have updated the foil for xs class to include all information needed on all the foils and isotopes
</commit_message>
<xml_diff>
--- a/A0_unc_persent.xlsx
+++ b/A0_unc_persent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{8E561148-20FF-1445-8691-D79058C33EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A2A6B98-0110-A34D-8B29-CE3A6D82DA72}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{8E561148-20FF-1445-8691-D79058C33EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70377499-F8DB-0648-A107-0D3FF9E9D596}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="20320" windowHeight="14920" xr2:uid="{F987D640-AF71-2948-8B84-AD1C60931213}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="20320" windowHeight="14420" xr2:uid="{F987D640-AF71-2948-8B84-AD1C60931213}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Zr01</t>
   </si>
@@ -162,6 +162,69 @@
   </si>
   <si>
     <t>60CO</t>
+  </si>
+  <si>
+    <t>60CU</t>
+  </si>
+  <si>
+    <t>61CU</t>
+  </si>
+  <si>
+    <t>64CU</t>
+  </si>
+  <si>
+    <t>56NI</t>
+  </si>
+  <si>
+    <t>57NI</t>
+  </si>
+  <si>
+    <t>65NI</t>
+  </si>
+  <si>
+    <t>59FE</t>
+  </si>
+  <si>
+    <t>Ti01</t>
+  </si>
+  <si>
+    <t>Ti02</t>
+  </si>
+  <si>
+    <t>Ti03</t>
+  </si>
+  <si>
+    <t>Ti04</t>
+  </si>
+  <si>
+    <t>Ti05</t>
+  </si>
+  <si>
+    <t>Ti06</t>
+  </si>
+  <si>
+    <t>Ti08</t>
+  </si>
+  <si>
+    <t>Ti09</t>
+  </si>
+  <si>
+    <t>Ti10</t>
+  </si>
+  <si>
+    <t>Ti11</t>
+  </si>
+  <si>
+    <t>46SC</t>
+  </si>
+  <si>
+    <t>47SC</t>
+  </si>
+  <si>
+    <t>48SC</t>
+  </si>
+  <si>
+    <t>48V</t>
   </si>
 </sst>
 </file>
@@ -534,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C214A759-CA15-BB43-B154-32249697E9E6}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,54 +825,106 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>